<commit_message>
een paar asset ideas
</commit_message>
<xml_diff>
--- a/AssetLists/Asset_List.xlsx
+++ b/AssetLists/Asset_List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>Deadline:</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Unwrap Character</t>
+  </si>
+  <si>
+    <t>1 hour, 40 minutes</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +737,9 @@
       <c r="F3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Thomas - Scene - Final
</commit_message>
<xml_diff>
--- a/AssetLists/Asset_List.xlsx
+++ b/AssetLists/Asset_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -823,7 +823,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1721,8 +1721,8 @@
       <c r="E32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="19" t="s">
-        <v>13</v>
+      <c r="F32" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5" t="s">

</xml_diff>